<commit_message>
Update GIS data and combined mapping
</commit_message>
<xml_diff>
--- a/Derived_Data/FOCB Monitoring Sites SHORT NAMES.xlsx
+++ b/Derived_Data/FOCB Monitoring Sites SHORT NAMES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Documents\State of the Bay 2020\Data\B8 Bay Water Quality\FOCB_WQ\Derived_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Documents\State of the Bay 2020\Data\B9. Nutrients\FOCB_Nutrients\Derived_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18408" windowHeight="6696"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Station_ID</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Orr's Island</t>
+  </si>
+  <si>
+    <t>Walton Park</t>
   </si>
 </sst>
 </file>
@@ -628,21 +631,21 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="3" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -665,7 +668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -693,7 +696,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -749,7 +752,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -776,7 +779,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -804,7 +807,7 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -832,7 +835,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -860,7 +863,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>48</v>
       </c>
@@ -888,7 +891,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -915,7 +918,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -942,7 +945,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -969,7 +972,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -996,7 +999,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1023,7 +1026,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1053,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1078,7 +1081,7 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -1106,7 +1109,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1134,7 +1137,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
@@ -1162,7 +1165,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
@@ -1190,7 +1193,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1218,7 +1221,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1246,7 +1249,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1274,7 +1277,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>

</xml_diff>